<commit_message>
refactor: update lecturer and student template files
</commit_message>
<xml_diff>
--- a/public/files/Create List Lecturers Template.xlsx
+++ b/public/files/Create List Lecturers Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C8F671-3FA3-47F1-ABFF-1868C741595E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBAAD60-60D5-44C5-845A-44798A93D437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -27,6 +24,9 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Full Name</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,16 +449,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: add new Excel templates for creating lecturers, students, and checklists
</commit_message>
<xml_diff>
--- a/public/files/Create List Lecturers Template.xlsx
+++ b/public/files/Create List Lecturers Template.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBAAD60-60D5-44C5-845A-44798A93D437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943A9308-6CF6-45D1-9620-8B9A65F577F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lecturers" sheetId="1" r:id="rId1"/>
+    <sheet name="Students" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -91,11 +91,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,16 +436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -463,21 +466,21 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="textLength" showErrorMessage="1" errorTitle="Invalid Name" error="Name must be between 2 and 100 characters." sqref="A2:A100 D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Name must be between 2 and 100 characters." sqref="A2:A1048576" xr:uid="{BC4B60E6-2BF2-4BA1-A9AF-1A01910E9095}">
       <formula1>2</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="custom" showErrorMessage="1" errorTitle="Invalid Email" error="Email must contain &quot;@&quot;." sqref="B2:B100" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Email" error="Email must contain &quot;@&quot;." sqref="B2:B1048576" xr:uid="{D816F5B6-6DE3-4736-872A-378854F19456}">
       <formula1>ISNUMBER(SEARCH("@",B2))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" showErrorMessage="1" errorTitle="Invalid Phone Number" error="Phone number must be 10 digits and start with 0." sqref="C2:C100" xr:uid="{00000000-0002-0000-0000-000065000000}">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Phone Number" error="Phone number must be 10 digits and start with 0." sqref="C2:C1048576" xr:uid="{D2AC175B-E4F0-452E-ABF7-C2A0BE6052CE}">
       <formula1>10</formula1>
     </dataValidation>
-    <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Gender" error="Gender must be either &quot;Male&quot; or &quot;Female&quot;." sqref="D3:D100" xr:uid="{00000000-0002-0000-0000-000067000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Gender" error="Gender must be either &quot;Male&quot; or &quot;Female&quot;." sqref="D2:D1048576" xr:uid="{799DB971-367B-4856-ABD1-3A6C9DA8BA14}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>